<commit_message>
Updated design document reorganized project struct
</commit_message>
<xml_diff>
--- a/schedule_worksplit/gantt_chart.xlsx
+++ b/schedule_worksplit/gantt_chart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16340" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="16500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -504,25 +504,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -540,9 +525,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -564,12 +546,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -588,55 +564,79 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -972,287 +972,287 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="180" workbookViewId="0">
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="9"/>
-    <col min="2" max="2" width="10.83203125" style="9" customWidth="1"/>
-    <col min="3" max="3" width="3.33203125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="4"/>
+    <col min="2" max="2" width="1" style="4" customWidth="1"/>
+    <col min="3" max="3" width="3.33203125" style="4" customWidth="1"/>
     <col min="4" max="4" width="27.83203125" style="1" customWidth="1"/>
     <col min="5" max="8" width="18" style="1" customWidth="1"/>
-    <col min="9" max="9" width="17" style="9" customWidth="1"/>
-    <col min="10" max="17" width="4.83203125" style="9" customWidth="1"/>
-    <col min="18" max="25" width="10.83203125" style="9"/>
+    <col min="9" max="9" width="17" style="4" customWidth="1"/>
+    <col min="10" max="17" width="4.83203125" style="4" customWidth="1"/>
+    <col min="18" max="25" width="10.83203125" style="4"/>
     <col min="26" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="3:9">
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
     </row>
     <row r="2" spans="3:9" ht="18" thickBot="1">
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
     </row>
     <row r="3" spans="3:9" ht="36" customHeight="1" thickTop="1" thickBot="1">
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="8"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="46"/>
     </row>
     <row r="4" spans="3:9" ht="22" thickTop="1">
-      <c r="C4" s="22"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="14" t="s">
+      <c r="C4" s="40"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="26" t="s">
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="18" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="3:9" ht="22" thickBot="1">
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="30"/>
-      <c r="E5" s="15" t="s">
+      <c r="D5" s="43"/>
+      <c r="E5" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="27" t="s">
+      <c r="I5" s="19" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="3:9" ht="3" customHeight="1" thickTop="1">
-      <c r="C6" s="17"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="12"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="7"/>
     </row>
     <row r="7" spans="3:9">
-      <c r="C7" s="17"/>
-      <c r="D7" s="19" t="s">
+      <c r="C7" s="11"/>
+      <c r="D7" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="29" t="s">
+      <c r="E7" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="12"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="7"/>
     </row>
     <row r="8" spans="3:9" ht="3" customHeight="1">
-      <c r="C8" s="17"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="12"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="7"/>
     </row>
     <row r="9" spans="3:9">
-      <c r="C9" s="17"/>
-      <c r="D9" s="19" t="s">
+      <c r="C9" s="11"/>
+      <c r="D9" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="29"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="12"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="7"/>
     </row>
     <row r="10" spans="3:9" ht="3" customHeight="1">
-      <c r="C10" s="17"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="12"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="7"/>
     </row>
     <row r="11" spans="3:9">
-      <c r="C11" s="17"/>
-      <c r="D11" s="20" t="s">
+      <c r="C11" s="11"/>
+      <c r="D11" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="37" t="s">
+      <c r="E11" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="12"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="7"/>
     </row>
     <row r="12" spans="3:9" ht="3" customHeight="1">
-      <c r="C12" s="17"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="12"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="7"/>
     </row>
     <row r="13" spans="3:9">
-      <c r="C13" s="17"/>
-      <c r="D13" s="20" t="s">
+      <c r="C13" s="11"/>
+      <c r="D13" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="38"/>
-      <c r="F13" s="39" t="s">
+      <c r="E13" s="28"/>
+      <c r="F13" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="39" t="s">
+      <c r="G13" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="H13" s="33"/>
-      <c r="I13" s="12"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="7"/>
     </row>
     <row r="14" spans="3:9" ht="3" customHeight="1">
-      <c r="C14" s="17"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="12"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="7"/>
     </row>
     <row r="15" spans="3:9">
-      <c r="C15" s="17"/>
-      <c r="D15" s="21" t="s">
+      <c r="C15" s="11"/>
+      <c r="D15" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="29"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="45"/>
-      <c r="I15" s="12"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="7"/>
     </row>
     <row r="16" spans="3:9" ht="3" customHeight="1">
-      <c r="C16" s="17"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="12"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="7"/>
     </row>
     <row r="17" spans="3:9">
-      <c r="C17" s="17"/>
-      <c r="D17" s="28" t="s">
+      <c r="C17" s="11"/>
+      <c r="D17" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="E17" s="37" t="s">
+      <c r="E17" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="12"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="7"/>
     </row>
     <row r="18" spans="3:9" ht="3" customHeight="1">
-      <c r="C18" s="17"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="12"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="7"/>
     </row>
     <row r="19" spans="3:9">
-      <c r="C19" s="17"/>
-      <c r="D19" s="28" t="s">
+      <c r="C19" s="11"/>
+      <c r="D19" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="38"/>
-      <c r="F19" s="39" t="s">
+      <c r="E19" s="28"/>
+      <c r="F19" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="G19" s="39" t="s">
+      <c r="G19" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="H19" s="46" t="s">
+      <c r="H19" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="I19" s="12"/>
+      <c r="I19" s="7"/>
     </row>
     <row r="20" spans="3:9" ht="3" customHeight="1">
-      <c r="C20" s="17"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="35"/>
-      <c r="I20" s="12"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="7"/>
     </row>
     <row r="21" spans="3:9" ht="16" customHeight="1">
-      <c r="C21" s="17"/>
-      <c r="D21" s="21" t="s">
+      <c r="C21" s="11"/>
+      <c r="D21" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E21" s="38"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="32"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="40" t="s">
+      <c r="E21" s="28"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="30" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="22" spans="3:9" ht="3" customHeight="1" thickBot="1">
-      <c r="C22" s="24"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="41"/>
-      <c r="F22" s="42"/>
-      <c r="G22" s="42"/>
-      <c r="H22" s="43"/>
-      <c r="I22" s="44"/>
-    </row>
-    <row r="23" spans="3:9" s="9" customFormat="1" ht="18" thickTop="1"/>
-    <row r="24" spans="3:9" s="9" customFormat="1"/>
-    <row r="25" spans="3:9" s="9" customFormat="1"/>
-    <row r="26" spans="3:9" s="9" customFormat="1"/>
-    <row r="27" spans="3:9" s="9" customFormat="1"/>
-    <row r="28" spans="3:9" s="9" customFormat="1"/>
-    <row r="29" spans="3:9" s="9" customFormat="1"/>
-    <row r="30" spans="3:9" s="9" customFormat="1"/>
-    <row r="31" spans="3:9" s="9" customFormat="1"/>
-    <row r="32" spans="3:9" s="9" customFormat="1"/>
-    <row r="33" s="9" customFormat="1"/>
-    <row r="34" s="9" customFormat="1"/>
-    <row r="35" s="9" customFormat="1"/>
-    <row r="36" s="9" customFormat="1"/>
-    <row r="37" s="9" customFormat="1"/>
-    <row r="38" s="9" customFormat="1"/>
-    <row r="39" s="9" customFormat="1"/>
-    <row r="40" s="9" customFormat="1"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="33"/>
+      <c r="I22" s="34"/>
+    </row>
+    <row r="23" spans="3:9" s="4" customFormat="1" ht="18" thickTop="1"/>
+    <row r="24" spans="3:9" s="4" customFormat="1"/>
+    <row r="25" spans="3:9" s="4" customFormat="1"/>
+    <row r="26" spans="3:9" s="4" customFormat="1"/>
+    <row r="27" spans="3:9" s="4" customFormat="1"/>
+    <row r="28" spans="3:9" s="4" customFormat="1"/>
+    <row r="29" spans="3:9" s="4" customFormat="1"/>
+    <row r="30" spans="3:9" s="4" customFormat="1"/>
+    <row r="31" spans="3:9" s="4" customFormat="1"/>
+    <row r="32" spans="3:9" s="4" customFormat="1"/>
+    <row r="33" s="4" customFormat="1"/>
+    <row r="34" s="4" customFormat="1"/>
+    <row r="35" s="4" customFormat="1"/>
+    <row r="36" s="4" customFormat="1"/>
+    <row r="37" s="4" customFormat="1"/>
+    <row r="38" s="4" customFormat="1"/>
+    <row r="39" s="4" customFormat="1"/>
+    <row r="40" s="4" customFormat="1"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="E4:H4"/>

</xml_diff>